<commit_message>
pushing new features to sheets
</commit_message>
<xml_diff>
--- a/inst/extdata/Template_info.xlsx
+++ b/inst/extdata/Template_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="456">
   <si>
     <t>dataset_name</t>
   </si>
@@ -134,10 +134,6 @@
   </si>
   <si>
     <t>other</t>
-  </si>
-  <si>
-    <t>author_year
-red font = required</t>
   </si>
   <si>
     <t>site_name</t>
@@ -1155,14 +1151,254 @@
     <t>f_ferrihydrite</t>
   </si>
   <si>
-    <t>This lorem ipsum generator is made for all the webdesigners, designers, webmasters and others who need lorem ipsum. Generator is made the way that everyone can use it, but especially for projects which need html markup. You can decide which html tags you want and our generator will generate just as you specified.</t>
+    <t xml:space="preserve">A unique name for a site that corresponds to a georeferenced point. </t>
+  </si>
+  <si>
+    <t>see metadata tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latitude/Longitude datum against which Latitude and Longitude are reported. If left blank, WGS84 will be assumed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Various notes on and descriptions of the site other than C flux, climate, photo or vegetation. May include local names for physiographic features, which may or may not appear on USGS Topographic Quadrangles. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The elevation at the site as determined by topo map, GPS, altimeter, etc. Contributed value is assumed accurate within several meters regardless of method used. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The angle of the ground surface through the site and in the direction that overland water would flow. Make observations facing downslope to avoid errors associated with some brands of clinometers. If the site has no slope leave blank. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cardinal direction that the slope faces at a site. Use this field if only if you do not provide the azimuth of the Site Aspect in compass degrees. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The numerical observation of aspect at the site. The compass bearing (corrected for declination) that a slope faces, looking downslope. If the site has no slope leave blank. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The geologic or organic precursors to the soil at the site </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The data contributor's calculated soil organic carbon stock value for the site, cluster, profile or layer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The arithmetic average of the total annual (liquid) precipitation , preferably taken over the standard "normal" period, 1961-1990. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The arithmetic average of the daily maximum and minimum temperatures for a calendar year, preferably taken over the standard "normal" period, 1961. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nation of origin of the data. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">State or territory. At output, may also include province for any contry that does not describe political subdivision as "states". </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provide references or links here if additional site-level vegetation data are available (e.g. species composition, basal area, aboveground biomass). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measure or estimate the depth from the ground surface to the stabilized contact with free- standing water in an open bore-hole or well at the time of sampling. </t>
+  </si>
+  <si>
+    <t>AGD84, ED50, ETRS89, GRS80, NAD83, OSGB36, WGS84</t>
+  </si>
+  <si>
+    <t>coastal mediterranean, dry winter, wet summer, highland climate, humid continental hot summer, wet all year, humid continental mild summer, dry winter, humid continental mild summer, wet all year, humid subtropical, ice cap, interior mediterranean, marine cool winter, marine mild wInter, mid-latitude dry arid desert, mid-latitude dry semiarid steppe, subarctic with cold winter, dry wInter, subarctic with cold winter, wet all year, subarctic with cool summer, dry winter, subarctic with cool summer, wet all year, subtropical dry arid desert, subtropical dry semiarid steppe, tropical monsoonal, tropical wet, tropical wet and dry, tundra</t>
+  </si>
+  <si>
+    <t>N, S, E, W, NE, NW, SE, SW</t>
+  </si>
+  <si>
+    <t>convergent, divergent, planar</t>
+  </si>
+  <si>
+    <t>boreal forest/taiga, desert or xeric shrubland, flooded grassland or savanna, mangrove, mediterranean forest, woodland, or scrub, montane grassland or shrubland, temperate broadleaf or mixed forest, temperate coniferous forest, temperate grassland, savanna and shrubland, tropical or subtropical coniferous forest, tropical or subtropical grassland, savanna, or shrubland, tropical or subtropical moist broadleaf forest, tundra</t>
+  </si>
+  <si>
+    <t>bare, cultivated, forest, rangeland/grassland, shrubland, urban, wetland</t>
+  </si>
+  <si>
+    <t>excessively, somewhat excessively, well, moderately well, somewhat poorly, poorly, very poorly</t>
+  </si>
+  <si>
+    <t>igneous intrusive, igneous extrusive, igneous pyroclastic, metamorphic, sedimentary-clastics, organic, evaporites, interbedded</t>
+  </si>
+  <si>
+    <t>mafic, felsic, intermediate</t>
+  </si>
+  <si>
+    <t>summit, shoulder, backslope, footslope, toeslope, interfluve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sand , loamy sand, sandy loam, loam, silt , silty loam, sandy clay loam, clay loam, silty clay loam, sandy clay, silty clay, clay </t>
+  </si>
+  <si>
+    <t>chloroform fumigation extraction, chloroform fumigation incubation, substrate induced respiration, total PLFA, other</t>
+  </si>
+  <si>
+    <t>SPT_Density, SPT_Density, HF, HF, Aggregate_Size, Aggregate_Size, Particle_Size, Incubation, Incubation</t>
+  </si>
+  <si>
+    <t>sonicated, soluble, insoluble, wet sieve, dry sieve, HMP, respired, not respired</t>
+  </si>
+  <si>
+    <t>see site tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A unique name for a single profile. This can be the same as the site name if there is only one profile at the site. For NRCS data it is the same as “Pedon ID”. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A unique name for a single sampled layer. This can be a name that denotes depth, sequence, etc. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The top (upper) depth of the layer. The surface of the non- green (i.e. non-living) surface layer is “0”. The top of the O- horizon should be 0. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The bottom (lower) depth of the layer. If it is uncertain that the bottom of the designated horizon was reached, enter the depth to the bottom of the sampled layer. Note that this is the same as "hzn_bot" in the NRCS database. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow conventions of the USDA-NRCS-NSSC Field Book for Describing and Sampling Soils (Staff 2002; pp. 2-2 through 2-4). Note that datasets originally using another convention will be modified for this column. If a different convention was used it can be entered in Horizon Designation Other. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The depth to which profiles were sampled to quantify the mean site, cluster, or profile calculated soil organic carbon stocks. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The standard deviation of the site, cluster, profile, or layer-level calculated soil organic carbon stock. (For layer soil organic carbon stocks, this may be based on analytical or sampling replicates of %C or bulk density measurements). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The data contributor's calculated soil organic carbon stock value for the profile </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The depth to the frozen surface of the profile. For Alaska sites, this applies only if sampled after August 15 and should be left blank if sampled before. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The observed depth to the top of the bedrock layer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The taxonomic classification of the soil profile following NRCS convention </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The NRCS soil series of the profile </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-dimensional position of the site on the Landform on which it is located. See USDA- NRCS-NSSC Field Book for Describing and Sampling Soils (Staff 2002; pp. 3-38 through 3-41). This information supplements Landscape and Landform to describe the geographic setting of the site. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Color of moist soil based on the Munsell soil color chart. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descriptive information indicating evidence of burning within the layer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grams of oven-dried soil per cubic centimeter, with soil particles greater than 2 mm and roots greater that 1 cm diameter removed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grams of oven-dried soil per cubic centimeter, with soil particles greater than 2 mm and roots greater that 1 cm diameter included. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please reference or describe the methods used to determine bulk density. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:2 soil-CaCl2 is the pH of a sample measured in 0.01M CaCl2 at a 1:2 soil:solution ratio. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:1 distilled water and soil paste. If pH was done by a different method, then enter it into one of the other soil pH fields. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH measurements other than 1:1 soil and distilled water paste or in CaCl2. Please document the method in the associated pH Method. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inorganic carbon concentration as measured or estimated by the contributor. Please document the method in the associated Processed Site Organic Carbon Content Method. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent by weight of soil particles greater than 0.05 mm in the sample remaining after removal of particles greater than 2 mm and roots greater than 1 cm diameter. See Gee, G.W. &amp; Bauder, J.W. 1986. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent by weight of soil particles in the size range from 0.002 to 0.050 mm in the sample remaining after removal of particles greater than 2 mm and roots greater than 1 cm diameter. See Gee, G.W. &amp; Bauder, J.W. 1986. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent by weight of soil particles less than 0.002 mm in the sample remaining after removal of particles greater than 2 mm and roots greater than 1 cm diameter. See Gee, G.W. &amp; Bauder, J.W. 1986. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cation Exchange Capacity. Document the extractant solution in the metadata worksheet, Lab Analysis Method. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soil texture classification. If no information is provided, this will be automatically generated from %sand, %silt, %clay data (coarse = ≥50% sand; fine = &lt;50% sand). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent by weight of nitrogen (organic and inorganic) in an oven-dried sample (the laboratory analytical concentration). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass ratio of total carbon to total nitrogen, as calculated from the total carbon and total nitrogen concentrations of the bulk layer, fraction, or other sample type. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent by weight of carbon in a dried soil sample after acidification with HCl, OR organic carbon as estimated by Walkley-Black Modified Acid-Dichromate (e.g. ‘Organic Carbon’ in the NRCS database). Please document the method in the associated Carbon Analysis Methods. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent by weight of carbon in the dried, milled soil sample. This measurement will typically correspond to analytical results from an elemental analyzer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A description of the methods used to calculate (including any gap-filling) site, cluster, profile or layer soil organic carbon stocks. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent by weight of the organic content of the &lt;2mm fraction is the organic material lost after ignition. It is reported on a &lt;2 mm base. Please document the method in the associated Carbon Analysis Method. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Per mille signature of δ15N relative to air (international standard). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Per mille signature of δ13C relative to Pee Dee Belemnite. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laboratory code for radiocarbon laboratory. Complete list of past and present laboratory codes can found published in Radiocarbon in November 2011  (http://www.radiocarbon.org/Info/labcodes.html). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year in which radiocarbon analysis was performed on the sample. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Layer sample identifier as designated by the radiocarbon laboratory. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Per mille signature of Δ14C relative to NBS Oxalic Acid standard. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error estimate for the fraction (eg. standard deviation of analytical reps). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deviation of the bulk sample or fraction from modern. Modern is defined as 95% of the radiocarbon concentration (in AD 1950) of NBS Oxalic Acid standard, 13C-corrected. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error estimate for an individual layer (eg. standard deviation of analytical reps). </t>
+  </si>
+  <si>
+    <t>see profile tab</t>
+  </si>
+  <si>
+    <t>see layer tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A unique name for a single fraction. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The scheme used to isolate the fraction, e.g., density, size, aggregate, chemical. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The value of the chemical or physical property that defines the fraction as unique from the others in its scheme, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The units of measurement of the property that defines a fraction as unique, e.g. for density fractions, "g cm-3". </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent by weight of nitrogen (organic and inorganic) in an oven- dried sample (the laboratory analytical concentration). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laboratory code for radiocarbon laboratory. Complete list of past and present laboratory codes can found published in Radiocarbon in November 2011 (http://www.radiocarbon.org/Info/labcodes.html). </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1198,6 +1434,11 @@
       <color rgb="FF666666"/>
       <name val="Tahoma"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="TimesNewRomanPSMT"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1216,23 +1457,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1565,7 +1835,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1725,10 +1995,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1737,7 +2007,7 @@
     <col min="2" max="2" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -1753,8 +2023,17 @@
       <c r="E1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1762,252 +2041,328 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="E6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>48</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>50</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>52</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>54</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>55</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>57</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>58</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>60</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>61</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>63</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>64</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>66</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>67</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>69</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>70</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="E15" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>72</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>73</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>75</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>76</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>78</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>79</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>81</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>82</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>84</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>85</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E20" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>87</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>88</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>90</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>91</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>93</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>94</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>96</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>97</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>99</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>100</v>
       </c>
-      <c r="C25" t="s">
-        <v>101</v>
+      <c r="D25" s="3" t="s">
+        <v>384</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2018,15 +2373,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C16385"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -2042,8 +2397,17 @@
       <c r="E1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2051,149 +2415,191 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>103</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>104</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>106</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>108</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>109</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>111</v>
-      </c>
-      <c r="B7" t="s">
-        <v>112</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
         <v>113</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>114</v>
       </c>
-      <c r="C8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>115</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>116</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="E9" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>118</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>120</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>122</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
         <v>123</v>
       </c>
-      <c r="C12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>124</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
         <v>125</v>
       </c>
-      <c r="C13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>126</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
         <v>127</v>
       </c>
-      <c r="C14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>128</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
         <v>129</v>
       </c>
-      <c r="C15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>130</v>
       </c>
-      <c r="B16" t="s">
-        <v>131</v>
-      </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -2208,15 +2614,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -2232,8 +2638,17 @@
       <c r="E1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2241,875 +2656,984 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>103</v>
       </c>
-      <c r="B4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
         <v>132</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>134</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>135</v>
       </c>
-      <c r="C6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>136</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
         <v>137</v>
       </c>
-      <c r="C7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>138</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>140</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>141</v>
       </c>
-      <c r="C9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>142</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>144</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" s="3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>146</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>147</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>149</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>150</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>152</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
         <v>153</v>
       </c>
-      <c r="C14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>154</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>156</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" s="3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>158</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" s="3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>160</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" s="3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>162</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
         <v>163</v>
       </c>
-      <c r="C19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>164</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
         <v>165</v>
       </c>
-      <c r="C20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>166</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
         <v>167</v>
       </c>
-      <c r="C21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>168</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
         <v>169</v>
       </c>
-      <c r="C22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>170</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
         <v>171</v>
       </c>
-      <c r="C23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>172</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>174</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>175</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="E25" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>177</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>179</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>180</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>182</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>183</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>185</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
         <v>186</v>
       </c>
-      <c r="C29" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>187</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
         <v>188</v>
       </c>
-      <c r="C30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>189</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
         <v>190</v>
       </c>
-      <c r="C31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
         <v>191</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
         <v>192</v>
       </c>
-      <c r="C32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
         <v>193</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
         <v>194</v>
       </c>
-      <c r="C33" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
         <v>195</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
         <v>196</v>
       </c>
-      <c r="C34" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
         <v>197</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
         <v>198</v>
       </c>
-      <c r="C35" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
         <v>199</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
         <v>200</v>
       </c>
-      <c r="C36" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
         <v>201</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>202</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" s="3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
         <v>204</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
         <v>205</v>
       </c>
-      <c r="C38" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
         <v>206</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>207</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" s="3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
         <v>209</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>207</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
         <v>210</v>
       </c>
-      <c r="C40" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
         <v>211</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>210</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
         <v>212</v>
       </c>
-      <c r="C41" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>213</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D42" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
         <v>215</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>216</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
         <v>218</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
+        <v>207</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
         <v>219</v>
       </c>
-      <c r="C44" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
         <v>220</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
         <v>221</v>
       </c>
-      <c r="C45" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
         <v>222</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
         <v>224</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D47" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
         <v>226</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>227</v>
       </c>
-      <c r="C48" t="s">
-        <v>228</v>
+      <c r="E48" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
+        <v>228</v>
+      </c>
+      <c r="B49" t="s">
         <v>229</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>230</v>
-      </c>
-      <c r="C49" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
+        <v>231</v>
+      </c>
+      <c r="B50" t="s">
         <v>232</v>
       </c>
-      <c r="B50" t="s">
-        <v>233</v>
-      </c>
       <c r="C50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
+        <v>233</v>
+      </c>
+      <c r="B51" t="s">
         <v>234</v>
-      </c>
-      <c r="B51" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
+        <v>235</v>
+      </c>
+      <c r="B52" t="s">
         <v>236</v>
-      </c>
-      <c r="B52" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
+        <v>237</v>
+      </c>
+      <c r="B53" t="s">
         <v>238</v>
-      </c>
-      <c r="B53" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
+        <v>239</v>
+      </c>
+      <c r="B54" t="s">
         <v>240</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>241</v>
-      </c>
-      <c r="C54" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
+        <v>242</v>
+      </c>
+      <c r="B55" t="s">
         <v>243</v>
       </c>
-      <c r="B55" t="s">
-        <v>244</v>
-      </c>
       <c r="C55" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>244</v>
+      </c>
+      <c r="B56" t="s">
         <v>245</v>
       </c>
-      <c r="B56" t="s">
-        <v>246</v>
-      </c>
       <c r="C56" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
+        <v>246</v>
+      </c>
+      <c r="B57" t="s">
         <v>247</v>
       </c>
-      <c r="B57" t="s">
-        <v>248</v>
-      </c>
       <c r="C57" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
+        <v>248</v>
+      </c>
+      <c r="B58" t="s">
         <v>249</v>
-      </c>
-      <c r="B58" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
+        <v>250</v>
+      </c>
+      <c r="B59" t="s">
         <v>251</v>
       </c>
-      <c r="B59" t="s">
-        <v>252</v>
-      </c>
       <c r="C59" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
+        <v>252</v>
+      </c>
+      <c r="B60" t="s">
         <v>253</v>
       </c>
-      <c r="B60" t="s">
-        <v>254</v>
-      </c>
       <c r="C60" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
+        <v>254</v>
+      </c>
+      <c r="B61" t="s">
         <v>255</v>
       </c>
-      <c r="B61" t="s">
-        <v>256</v>
-      </c>
       <c r="C61" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
+        <v>256</v>
+      </c>
+      <c r="B62" t="s">
         <v>257</v>
       </c>
-      <c r="B62" t="s">
-        <v>258</v>
-      </c>
       <c r="C62" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
+        <v>258</v>
+      </c>
+      <c r="B63" t="s">
         <v>259</v>
-      </c>
-      <c r="B63" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
+        <v>260</v>
+      </c>
+      <c r="B64" t="s">
         <v>261</v>
       </c>
-      <c r="B64" t="s">
-        <v>262</v>
-      </c>
       <c r="C64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
+        <v>262</v>
+      </c>
+      <c r="B65" t="s">
         <v>263</v>
       </c>
-      <c r="B65" t="s">
-        <v>264</v>
-      </c>
       <c r="C65" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
+        <v>264</v>
+      </c>
+      <c r="B66" t="s">
         <v>265</v>
       </c>
-      <c r="B66" t="s">
-        <v>266</v>
-      </c>
       <c r="C66" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
+        <v>266</v>
+      </c>
+      <c r="B67" t="s">
         <v>267</v>
       </c>
-      <c r="B67" t="s">
-        <v>268</v>
-      </c>
       <c r="C67" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
+        <v>268</v>
+      </c>
+      <c r="B68" t="s">
         <v>269</v>
       </c>
-      <c r="B68" t="s">
-        <v>270</v>
-      </c>
       <c r="C68" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
+        <v>270</v>
+      </c>
+      <c r="B69" t="s">
         <v>271</v>
       </c>
-      <c r="B69" t="s">
-        <v>272</v>
-      </c>
       <c r="C69" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
+        <v>272</v>
+      </c>
+      <c r="B70" t="s">
         <v>273</v>
       </c>
-      <c r="B70" t="s">
-        <v>274</v>
-      </c>
       <c r="C70" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
+        <v>274</v>
+      </c>
+      <c r="B71" t="s">
         <v>275</v>
       </c>
-      <c r="B71" t="s">
-        <v>276</v>
-      </c>
       <c r="C71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
+        <v>276</v>
+      </c>
+      <c r="B72" t="s">
         <v>277</v>
       </c>
-      <c r="B72" t="s">
-        <v>278</v>
-      </c>
       <c r="C72" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
+        <v>278</v>
+      </c>
+      <c r="B73" t="s">
         <v>279</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>280</v>
-      </c>
-      <c r="C73" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
+        <v>281</v>
+      </c>
+      <c r="B74" t="s">
         <v>282</v>
       </c>
-      <c r="B74" t="s">
-        <v>283</v>
-      </c>
       <c r="C74" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
+        <v>283</v>
+      </c>
+      <c r="B75" t="s">
         <v>284</v>
       </c>
-      <c r="B75" t="s">
-        <v>285</v>
-      </c>
       <c r="C75" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
+        <v>285</v>
+      </c>
+      <c r="B76" t="s">
         <v>286</v>
       </c>
-      <c r="B76" t="s">
-        <v>287</v>
-      </c>
       <c r="C76" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
+        <v>287</v>
+      </c>
+      <c r="B77" t="s">
         <v>288</v>
       </c>
-      <c r="B77" t="s">
-        <v>289</v>
-      </c>
       <c r="C77" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
+        <v>289</v>
+      </c>
+      <c r="B78" t="s">
         <v>290</v>
       </c>
-      <c r="B78" t="s">
-        <v>291</v>
-      </c>
       <c r="C78" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
+        <v>291</v>
+      </c>
+      <c r="B79" t="s">
         <v>292</v>
       </c>
-      <c r="B79" t="s">
-        <v>293</v>
-      </c>
       <c r="C79" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
+        <v>293</v>
+      </c>
+      <c r="B80" t="s">
         <v>294</v>
       </c>
-      <c r="B80" t="s">
-        <v>295</v>
-      </c>
       <c r="C80" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
+        <v>295</v>
+      </c>
+      <c r="B81" t="s">
         <v>296</v>
       </c>
-      <c r="B81" t="s">
-        <v>297</v>
-      </c>
       <c r="C81" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
+        <v>297</v>
+      </c>
+      <c r="B82" t="s">
         <v>298</v>
       </c>
-      <c r="B82" t="s">
-        <v>299</v>
-      </c>
       <c r="C82" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
+        <v>299</v>
+      </c>
+      <c r="B83" t="s">
         <v>300</v>
       </c>
-      <c r="B83" t="s">
-        <v>301</v>
-      </c>
       <c r="C83" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
+        <v>301</v>
+      </c>
+      <c r="B84" t="s">
         <v>302</v>
       </c>
-      <c r="B84" t="s">
-        <v>303</v>
-      </c>
       <c r="C84" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
+        <v>303</v>
+      </c>
+      <c r="B85" t="s">
         <v>304</v>
       </c>
-      <c r="B85" t="s">
-        <v>305</v>
-      </c>
       <c r="C85" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
+        <v>305</v>
+      </c>
+      <c r="B86" t="s">
         <v>306</v>
       </c>
-      <c r="B86" t="s">
-        <v>307</v>
-      </c>
       <c r="C86" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3120,15 +3644,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -3144,8 +3671,17 @@
       <c r="E1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17">
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3153,449 +3689,515 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17">
+    <row r="3" spans="1:8" ht="17">
       <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="D3" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
         <v>103</v>
       </c>
-      <c r="B4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
         <v>132</v>
       </c>
-      <c r="B5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="D5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B6" t="s">
         <v>308</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>310</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>311</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="E7" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>313</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>314</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="E8" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>316</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>317</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>319</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>321</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>323</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>324</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>326</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
         <v>327</v>
       </c>
-      <c r="C13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>328</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>330</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
         <v>331</v>
       </c>
-      <c r="C15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>332</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>334</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>335</v>
       </c>
-      <c r="C17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>336</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>337</v>
       </c>
-      <c r="C18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>338</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>339</v>
       </c>
-      <c r="C19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>340</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>341</v>
       </c>
-      <c r="C20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>342</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>343</v>
       </c>
-      <c r="C21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>344</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" s="3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>346</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>207</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
         <v>347</v>
       </c>
-      <c r="C23" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>348</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
         <v>349</v>
       </c>
-      <c r="C24" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>211</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
         <v>350</v>
       </c>
-      <c r="B25" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
+        <v>213</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
         <v>351</v>
       </c>
-      <c r="B26" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
+        <v>215</v>
+      </c>
+      <c r="C27" t="s">
+        <v>216</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
         <v>352</v>
       </c>
-      <c r="B27" t="s">
-        <v>216</v>
-      </c>
-      <c r="C27" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>353</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>207</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
         <v>354</v>
       </c>
-      <c r="C28" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>355</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>207</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
         <v>356</v>
       </c>
-      <c r="C29" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>357</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>359</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>361</v>
-      </c>
       <c r="B32" t="s">
+        <v>279</v>
+      </c>
+      <c r="C32" t="s">
         <v>280</v>
-      </c>
-      <c r="C32" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>363</v>
+      </c>
+      <c r="B35" t="s">
         <v>364</v>
       </c>
-      <c r="B35" t="s">
-        <v>365</v>
-      </c>
       <c r="C35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B36" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C36" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B37" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B38" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C38" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B39" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B40" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C40" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B41" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B42" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C42" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B43" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C43" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B44" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C44" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B45" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C45" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>